<commit_message>
todas las pestañas hechas
</commit_message>
<xml_diff>
--- a/app/uploads/Prueba asignar camas.xlsx
+++ b/app/uploads/Prueba asignar camas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>nombre_alumno</t>
   </si>
@@ -41,6 +41,36 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>apellido1</t>
+  </si>
+  <si>
+    <t>apellido2</t>
+  </si>
+  <si>
+    <t>brigada</t>
+  </si>
+  <si>
+    <t>especialidad</t>
+  </si>
+  <si>
+    <t>martinez</t>
+  </si>
+  <si>
+    <t>soriano</t>
+  </si>
+  <si>
+    <t>hernandez</t>
+  </si>
+  <si>
+    <t>de zuloaga</t>
+  </si>
+  <si>
+    <t>oss</t>
+  </si>
+  <si>
+    <t>ham</t>
   </si>
 </sst>
 </file>
@@ -382,48 +412,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>400</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>401</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>